<commit_message>
Added XlScriptReaderContext and skipScript option
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/xlscript/Test.xlsx
+++ b/src/test/resources/org/xlbean/xlscript/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\xldsl\xlscript\src\test\resources\org\xlbean\xlscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D4BA7D-80E2-4D39-B2A7-7907E90C8612}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9297DE76-A8FF-4944-8FF6-6E3D57137BC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21780" yWindow="0" windowWidth="21924" windowHeight="8652" activeTab="1" xr2:uid="{45094189-5854-4264-84B2-85A9732F2E97}"/>
+    <workbookView xWindow="4824" yWindow="2256" windowWidth="21948" windowHeight="12660" activeTab="1" xr2:uid="{45094189-5854-4264-84B2-85A9732F2E97}"/>
   </bookViews>
   <sheets>
     <sheet name="tableAndFlat" sheetId="1" r:id="rId1"/>
@@ -141,10 +141,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>list#key?toBean=key</t>
-  </si>
-  <si>
-    <t>list#value?toBean=value</t>
+    <t>list#key?toMap=key</t>
+  </si>
+  <si>
+    <t>list#value?toMap=value</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added unit tests and logs
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/xlscript/Test.xlsx
+++ b/src/test/resources/org/xlbean/xlscript/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\xldsl\xlscript\src\test\resources\org\xlbean\xlscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9297DE76-A8FF-4944-8FF6-6E3D57137BC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97F95AC-F7D1-4212-A587-9BC4AD0FEEF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4824" yWindow="2256" windowWidth="21948" windowHeight="12660" activeTab="1" xr2:uid="{45094189-5854-4264-84B2-85A9732F2E97}"/>
+    <workbookView xWindow="1344" yWindow="-108" windowWidth="29484" windowHeight="17496" activeTab="1" xr2:uid="{45094189-5854-4264-84B2-85A9732F2E97}"/>
   </bookViews>
   <sheets>
     <sheet name="tableAndFlat" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -145,6 +145,10 @@
   </si>
   <si>
     <t>list#value?toMap=value</t>
+  </si>
+  <si>
+    <t>aaa.bbb</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -627,10 +631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EAFB78-2A2A-4CBA-B81C-5FEFBBA0573F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -639,7 +643,7 @@
     <col min="4" max="4" width="25.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -649,8 +653,11 @@
       <c r="D1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -661,7 +668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>18</v>
       </c>
@@ -669,12 +676,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>